<commit_message>
t # This is a combination of 2 commits.
more keymap updates
</commit_message>
<xml_diff>
--- a/app/boards/shields/sofle/sofle_keymaps.xlsx
+++ b/app/boards/shields/sofle/sofle_keymaps.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" state="visible" r:id="rId3"/>
@@ -332,190 +332,190 @@
     <t xml:space="preserve">mkp MCLK</t>
   </si>
   <si>
+    <t xml:space="preserve">kp PG_DN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp LEFT_BRACKET   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp RIGHT_BRACKET   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp END   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp PSCRN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">none       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp INS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_NUM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_DIVIDE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_MULTIPLY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_MINUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp BACKSLASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp CLCK                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp UP      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N8     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N9       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_PLUS  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp DEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp LEFT    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp DOWN    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp RIGHT      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N5     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N6       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp K_UNDO  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp K_CUT   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp K_COPY     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp K_PASTE    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N2     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N3       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_ENTER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp KP_N0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_CLR        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_SEL 0    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_SEL 1    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_SEL 2    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_SEL 3    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_SEL 4     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_DISC 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_DISC 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_DISC 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_DISC 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bt BT_DISC 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">soft_off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext_power EP_TOG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_HUD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_HUI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_SAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_SAI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_EFF  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_TOG   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_BRD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_BRI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_SPI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_SPD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_EFR  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">none           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">none            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb_ug RGB_TOG             </t>
+  </si>
+  <si>
     <t xml:space="preserve">kp C_MUTE        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_TOG             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp PG_DN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp LEFT_BRACKET   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp RIGHT_BRACKET   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp END   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp PSCRN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">none       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp INS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_NUM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_DIVIDE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_MULTIPLY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_MINUS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp BACKSLASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp CLCK                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp UP      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N7  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N8     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N9       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_PLUS  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp DEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp LEFT    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp DOWN    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp RIGHT      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N4  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N5     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N6       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp K_UNDO  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp K_CUT   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp K_COPY     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp K_PASTE    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N2     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N3       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_ENTER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kp KP_N0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_CLR        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_SEL 0    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_SEL 1    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_SEL 2    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_SEL 3    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_SEL 4     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_DISC 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_DISC 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_DISC 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_DISC 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bt BT_DISC 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">soft_off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ext_power EP_TOG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_HUD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_HUI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_SAD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_SAI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_EFF  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_TOG   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_BRD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_BRI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_SPI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_SPD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb_ug RGB_EFR  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">none           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">none            </t>
   </si>
   <si>
     <t xml:space="preserve">out OUT_USB    </t>
@@ -531,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -559,11 +559,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -608,7 +603,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -618,10 +613,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1008,8 +999,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1194,7 +1185,7 @@
       <c r="G5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1450,22 +1441,22 @@
         <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>14</v>
@@ -1494,7 +1485,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>100</v>
@@ -1524,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1576,13 +1567,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>90</v>
@@ -1594,36 +1585,36 @@
         <v>92</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1635,36 +1626,36 @@
         <v>93</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
@@ -1673,16 +1664,16 @@
         <v>99</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>14</v>
@@ -1693,40 +1684,40 @@
         <v>100</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>100</v>
@@ -1752,10 +1743,10 @@
         <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>100</v>
@@ -1783,7 +1774,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1834,60 +1825,60 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>89</v>
@@ -1905,27 +1896,27 @@
         <v>89</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>89</v>
@@ -1943,7 +1934,7 @@
         <v>89</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,25 +1942,25 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>89</v>
@@ -1987,15 +1978,15 @@
         <v>89</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
swap alt and rl
</commit_message>
<xml_diff>
--- a/app/boards/shields/sofle/sofle_keymaps.xlsx
+++ b/app/boards/shields/sofle/sofle_keymaps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="166">
   <si>
     <t xml:space="preserve">c0</t>
   </si>
@@ -230,12 +230,12 @@
     <t xml:space="preserve">kp LCTRL </t>
   </si>
   <si>
+    <t xml:space="preserve">kp LALT </t>
+  </si>
+  <si>
     <t xml:space="preserve">mo LOWER  </t>
   </si>
   <si>
-    <t xml:space="preserve">kp LALT </t>
-  </si>
-  <si>
     <t xml:space="preserve">kp SPACE    </t>
   </si>
   <si>
@@ -248,10 +248,10 @@
     <t xml:space="preserve">kp RET           </t>
   </si>
   <si>
+    <t xml:space="preserve">mo RAISE  </t>
+  </si>
+  <si>
     <t xml:space="preserve">kp RALT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mo RAISE  </t>
   </si>
   <si>
     <t xml:space="preserve">kp RCTRL</t>
@@ -741,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1774,7 +1774,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2008,6 +2008,9 @@
       </c>
       <c r="K6" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more map updates/encoder tweaks
</commit_message>
<xml_diff>
--- a/app/boards/shields/sofle/sofle_keymaps.xlsx
+++ b/app/boards/shields/sofle/sofle_keymaps.xlsx
@@ -1002,8 +1002,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q38" activeCellId="0" sqref="Q38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1749,13 +1749,13 @@
         <v>107</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="L6" s="2" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1777,7 +1777,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>